<commit_message>
Add "literal" word and refactor findByName methods
Added "literal" word type to enable specific behavior for literal numbers within the Forth-like language architecture. Refactored findByName methods in WordService and DictionaryService to directly return "Word" rather than "Optional<Word>". This simplifies the code and improves readability. Removed unneeded verbose logging and comments.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="287">
   <si>
     <t xml:space="preserve">Forth-79</t>
   </si>
@@ -184,73 +184,79 @@
     <t xml:space="preserve">+ORIGIN</t>
   </si>
   <si>
+    <t xml:space="preserve">;</t>
+  </si>
+  <si>
     <t xml:space="preserve">2SWAP</t>
   </si>
   <si>
-    <t xml:space="preserve">;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;#</t>
+  </si>
+  <si>
     <t xml:space="preserve">--&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;#</t>
+    <t xml:space="preserve">&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">-DUP</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;</t>
+    <t xml:space="preserve">&gt;IN</t>
   </si>
   <si>
     <t xml:space="preserve">-FIND</t>
   </si>
   <si>
+    <t xml:space="preserve">&gt;R</t>
+  </si>
+  <si>
     <t xml:space="preserve">&gt;BODY</t>
   </si>
   <si>
     <t xml:space="preserve">-LINE</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;R</t>
-  </si>
-  <si>
     <t xml:space="preserve">?</t>
   </si>
   <si>
     <t xml:space="preserve">?DUP</t>
   </si>
   <si>
+    <t xml:space="preserve">@</t>
+  </si>
+  <si>
     <t xml:space="preserve">&gt;NUMBER</t>
   </si>
   <si>
-    <t xml:space="preserve">@</t>
+    <t xml:space="preserve">[</t>
   </si>
   <si>
     <t xml:space="preserve">.R</t>
   </si>
   <si>
-    <t xml:space="preserve">[</t>
+    <t xml:space="preserve">[COMPILE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">]</t>
   </si>
   <si>
     <t xml:space="preserve">[']</t>
   </si>
   <si>
-    <t xml:space="preserve">[COMPILE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">]</t>
+    <t xml:space="preserve">ABORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABS</t>
   </si>
   <si>
     <t xml:space="preserve">MOD</t>
   </si>
   <si>
-    <t xml:space="preserve">ABORT</t>
+    <t xml:space="preserve">ALLOT</t>
   </si>
   <si>
     <t xml:space="preserve">[CHAR]</t>
@@ -259,25 +265,22 @@
     <t xml:space="preserve">0BRANCH</t>
   </si>
   <si>
-    <t xml:space="preserve">ABS</t>
+    <t xml:space="preserve">AND</t>
   </si>
   <si>
     <t xml:space="preserve">ABORT"</t>
   </si>
   <si>
-    <t xml:space="preserve">ALLOT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AND</t>
-  </si>
-  <si>
     <t xml:space="preserve">BASE</t>
   </si>
   <si>
+    <t xml:space="preserve">BEGIN</t>
+  </si>
+  <si>
     <t xml:space="preserve">;CODE</t>
   </si>
   <si>
-    <t xml:space="preserve">BEGIN</t>
+    <t xml:space="preserve">BLK</t>
   </si>
   <si>
     <t xml:space="preserve">ACCEPT</t>
@@ -286,33 +289,36 @@
     <t xml:space="preserve">;S</t>
   </si>
   <si>
-    <t xml:space="preserve">BLK</t>
+    <t xml:space="preserve">BLOCK</t>
   </si>
   <si>
     <t xml:space="preserve">ALIGN</t>
   </si>
   <si>
-    <t xml:space="preserve">BLOCK</t>
+    <t xml:space="preserve">BUFFER</t>
   </si>
   <si>
     <t xml:space="preserve">ALIGNED</t>
   </si>
   <si>
-    <t xml:space="preserve">BUFFER</t>
+    <t xml:space="preserve">C!</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;BUILDS</t>
   </si>
   <si>
-    <t xml:space="preserve">C!</t>
-  </si>
-  <si>
     <t xml:space="preserve">C@</t>
   </si>
   <si>
     <t xml:space="preserve">CMOVE</t>
   </si>
   <si>
+    <t xml:space="preserve">COLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPILE</t>
+  </si>
+  <si>
     <t xml:space="preserve">CMOVE&gt;</t>
   </si>
   <si>
@@ -322,24 +328,21 @@
     <t xml:space="preserve">?COMP</t>
   </si>
   <si>
-    <t xml:space="preserve">COLON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPILE</t>
+    <t xml:space="preserve">CONSTANT</t>
   </si>
   <si>
     <t xml:space="preserve">?CSP</t>
   </si>
   <si>
-    <t xml:space="preserve">CONSTANT</t>
-  </si>
-  <si>
     <t xml:space="preserve">C,</t>
   </si>
   <si>
     <t xml:space="preserve">?EXEC</t>
   </si>
   <si>
+    <t xml:space="preserve">CONTEXT</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONVERT</t>
   </si>
   <si>
@@ -355,9 +358,6 @@
     <t xml:space="preserve">?PAIRS</t>
   </si>
   <si>
-    <t xml:space="preserve">CONTEXT</t>
-  </si>
-  <si>
     <t xml:space="preserve">CR</t>
   </si>
   <si>
@@ -382,6 +382,9 @@
     <t xml:space="preserve">CHAR+</t>
   </si>
   <si>
+    <t xml:space="preserve">CURRENT</t>
+  </si>
+  <si>
     <t xml:space="preserve">D&lt;</t>
   </si>
   <si>
@@ -391,9 +394,6 @@
     <t xml:space="preserve">DECIMAL</t>
   </si>
   <si>
-    <t xml:space="preserve">CURRENT</t>
-  </si>
-  <si>
     <t xml:space="preserve">DEFINITIONS</t>
   </si>
   <si>
@@ -439,6 +439,9 @@
     <t xml:space="preserve">EXIT</t>
   </si>
   <si>
+    <t xml:space="preserve">EMPTY-BUFFERS</t>
+  </si>
+  <si>
     <t xml:space="preserve">EXPECT</t>
   </si>
   <si>
@@ -454,9 +457,6 @@
     <t xml:space="preserve">BLANKS</t>
   </si>
   <si>
-    <t xml:space="preserve">EMPTY-BUFFERS</t>
-  </si>
-  <si>
     <t xml:space="preserve">FIND</t>
   </si>
   <si>
@@ -520,15 +520,15 @@
     <t xml:space="preserve">LITERAL</t>
   </si>
   <si>
+    <t xml:space="preserve">LIST</t>
+  </si>
+  <si>
     <t xml:space="preserve">LOAD</t>
   </si>
   <si>
     <t xml:space="preserve">LOOP</t>
   </si>
   <si>
-    <t xml:space="preserve">LIST</t>
-  </si>
-  <si>
     <t xml:space="preserve">MAX</t>
   </si>
   <si>
@@ -553,12 +553,12 @@
     <t xml:space="preserve">D+-</t>
   </si>
   <si>
+    <t xml:space="preserve">MOVE</t>
+  </si>
+  <si>
     <t xml:space="preserve">OR</t>
   </si>
   <si>
-    <t xml:space="preserve">MOVE</t>
-  </si>
-  <si>
     <t xml:space="preserve">D.</t>
   </si>
   <si>
@@ -595,6 +595,9 @@
     <t xml:space="preserve">DLIST</t>
   </si>
   <si>
+    <t xml:space="preserve">QUERY</t>
+  </si>
+  <si>
     <t xml:space="preserve">REPEAT</t>
   </si>
   <si>
@@ -610,9 +613,6 @@
     <t xml:space="preserve">DMINUS</t>
   </si>
   <si>
-    <t xml:space="preserve">QUERY</t>
-  </si>
-  <si>
     <t xml:space="preserve">ROT</t>
   </si>
   <si>
@@ -649,6 +649,9 @@
     <t xml:space="preserve">DR0</t>
   </si>
   <si>
+    <t xml:space="preserve">SCR</t>
+  </si>
+  <si>
     <t xml:space="preserve">STATE</t>
   </si>
   <si>
@@ -658,24 +661,21 @@
     <t xml:space="preserve">DR1</t>
   </si>
   <si>
+    <t xml:space="preserve">SEMICOLON</t>
+  </si>
+  <si>
     <t xml:space="preserve">SWAP</t>
   </si>
   <si>
     <t xml:space="preserve">SOURCE</t>
   </si>
   <si>
-    <t xml:space="preserve">SCR</t>
-  </si>
-  <si>
     <t xml:space="preserve">THEN</t>
   </si>
   <si>
     <t xml:space="preserve">DUMP</t>
   </si>
   <si>
-    <t xml:space="preserve">SEMICOLON</t>
-  </si>
-  <si>
     <t xml:space="preserve">TIB</t>
   </si>
   <si>
@@ -706,6 +706,9 @@
     <t xml:space="preserve">ENDIF</t>
   </si>
   <si>
+    <t xml:space="preserve">U*</t>
+  </si>
+  <si>
     <t xml:space="preserve">UPDATE</t>
   </si>
   <si>
@@ -718,7 +721,7 @@
     <t xml:space="preserve">ERROR</t>
   </si>
   <si>
-    <t xml:space="preserve">U*</t>
+    <t xml:space="preserve">U/</t>
   </si>
   <si>
     <t xml:space="preserve">VOCABULARY</t>
@@ -728,9 +731,6 @@
   </si>
   <si>
     <t xml:space="preserve">WHILE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U/</t>
   </si>
   <si>
     <t xml:space="preserve">WORD</t>
@@ -1012,11 +1012,11 @@
   </sheetPr>
   <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D168" activeCellId="0" sqref="D168"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="2" sqref="A30 B31 C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1431,7 +1431,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1445,27 +1445,27 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="C31" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="0" t="s">
+      <c r="A32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1474,69 +1474,69 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>55</v>
+      <c r="C33" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>60</v>
+      <c r="A36" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>25</v>
@@ -1544,13 +1544,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>23</v>
@@ -1558,13 +1558,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>67</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>26</v>
@@ -1572,24 +1572,24 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>67</v>
@@ -1600,13 +1600,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>30</v>
@@ -1614,13 +1614,13 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>33</v>
@@ -1628,13 +1628,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>35</v>
@@ -1642,27 +1642,27 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>37</v>
@@ -1670,13 +1670,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>43</v>
@@ -1684,55 +1684,55 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>55</v>
+      <c r="D48" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>83</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>56</v>
@@ -1740,49 +1740,49 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>95</v>
@@ -1791,18 +1791,18 @@
         <v>83</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>96</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>66</v>
@@ -1810,38 +1810,38 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>104</v>
@@ -1852,35 +1852,35 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>95</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>112</v>
@@ -1893,8 +1893,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>106</v>
+      <c r="A63" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>115</v>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>118</v>
@@ -1917,54 +1917,54 @@
         <v>119</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
-        <v>112</v>
+      <c r="A65" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>124</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>125</v>
@@ -1973,12 +1973,12 @@
         <v>112</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>126</v>
@@ -1987,18 +1987,18 @@
         <v>115</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>127</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>128</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>129</v>
@@ -2015,12 +2015,12 @@
         <v>125</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>130</v>
@@ -2029,12 +2029,12 @@
         <v>127</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>131</v>
@@ -2048,7 +2048,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>133</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>135</v>
@@ -2076,7 +2076,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>137</v>
@@ -2089,8 +2089,8 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>131</v>
+      <c r="A77" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>138</v>
@@ -2099,40 +2099,40 @@
         <v>135</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="s">
-        <v>135</v>
+      <c r="A79" s="0" t="s">
+        <v>137</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>145</v>
@@ -2141,12 +2141,12 @@
         <v>137</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>146</v>
@@ -2155,18 +2155,18 @@
         <v>138</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>147</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>148</v>
@@ -2174,7 +2174,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>149</v>
@@ -2188,7 +2188,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>151</v>
@@ -2202,7 +2202,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>154</v>
@@ -2211,12 +2211,12 @@
         <v>154</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>155</v>
@@ -2225,12 +2225,12 @@
         <v>155</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>156</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>157</v>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>158</v>
@@ -2272,7 +2272,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>160</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>162</v>
@@ -2300,7 +2300,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>164</v>
@@ -2309,54 +2309,54 @@
         <v>162</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B93" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>164</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C94" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>165</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
-        <v>164</v>
+      <c r="A95" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>169</v>
@@ -2370,7 +2370,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>171</v>
@@ -2384,10 +2384,10 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>169</v>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>174</v>
@@ -2412,13 +2412,13 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>169</v>
+        <v>77</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>175</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>176</v>
@@ -2426,13 +2426,13 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B101" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C101" s="0" t="s">
         <v>177</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>178</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>179</v>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>75</v>
+        <v>174</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>180</v>
@@ -2454,13 +2454,13 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>182</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>183</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>184</v>
@@ -2477,12 +2477,12 @@
         <v>180</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>185</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>187</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>189</v>
@@ -2524,41 +2524,41 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>189</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>197</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>127</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>198</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>199</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B113" s="0" t="s">
         <v>201</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B114" s="0" t="s">
         <v>204</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B115" s="0" t="s">
         <v>207</v>
@@ -2636,27 +2636,27 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D117" s="0" t="s">
         <v>130</v>
@@ -2664,21 +2664,21 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C118" s="0" t="s">
         <v>201</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>218</v>
@@ -2692,13 +2692,13 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>219</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D120" s="0" t="s">
         <v>133</v>
@@ -2706,13 +2706,13 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>220</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>135</v>
@@ -2720,21 +2720,21 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="B122" s="0" t="s">
         <v>221</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="B123" s="0" t="s">
         <v>222</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B124" s="0" t="s">
         <v>224</v>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B125" s="0" t="s">
         <v>226</v>
@@ -2776,52 +2776,52 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C126" s="0" t="s">
         <v>222</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C127" s="0" t="s">
         <v>224</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="D128" s="0" t="s">
         <v>232</v>
-      </c>
-      <c r="B128" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C128" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D128" s="0" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C129" s="0" t="s">
         <v>226</v>
@@ -2832,27 +2832,27 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>237</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>238</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D131" s="0" t="s">
         <v>239</v>
@@ -2860,7 +2860,7 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>240</v>
@@ -2869,12 +2869,12 @@
         <v>237</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C133" s="0" t="s">
         <v>238</v>
@@ -2885,7 +2885,7 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>240</v>
@@ -2896,32 +2896,26 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
-        <v>237</v>
+      <c r="A136" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="D136" s="0" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
-        <v>238</v>
-      </c>
       <c r="D137" s="0" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="D138" s="0" t="s">
         <v>243</v>
       </c>
@@ -2998,7 +2992,7 @@
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D153" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3007,18 +3001,18 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D155" s="0" t="s">
+      <c r="D155" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D156" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D157" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,7 +3052,7 @@
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D165" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,7 +3062,7 @@
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D167" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3093,7 +3087,7 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D172" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3138,7 +3132,7 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D181" s="0" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3173,7 +3167,7 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D188" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3193,7 +3187,7 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D192" s="0" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,12 +3222,12 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D199" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D200" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3248,7 +3242,7 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D203" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3278,12 +3272,12 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D209" s="0" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D210" s="0" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3293,7 +3287,7 @@
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D212" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3308,7 +3302,7 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D215" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3323,7 +3317,7 @@
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D218" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3333,7 +3327,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D220" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add 'spaces' primitive word and update CoreForth4j.sql
Added the 'spaces' primitive word to the core definitions in CoreDefinitions.groovy and updated CoreForth4j.sql file. The script now has a more succinct syntax and was streamlined for efficiency.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="287">
   <si>
     <t xml:space="preserve">Forth-79</t>
   </si>
@@ -700,28 +700,28 @@
     <t xml:space="preserve">END</t>
   </si>
   <si>
+    <t xml:space="preserve">U*</t>
+  </si>
+  <si>
     <t xml:space="preserve">UNTIL</t>
   </si>
   <si>
     <t xml:space="preserve">ENDIF</t>
   </si>
   <si>
-    <t xml:space="preserve">U*</t>
-  </si>
-  <si>
     <t xml:space="preserve">UPDATE</t>
   </si>
   <si>
     <t xml:space="preserve">ERASE</t>
   </si>
   <si>
+    <t xml:space="preserve">U/</t>
+  </si>
+  <si>
     <t xml:space="preserve">VARIABLE</t>
   </si>
   <si>
     <t xml:space="preserve">ERROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U/</t>
   </si>
   <si>
     <t xml:space="preserve">VOCABULARY</t>
@@ -1012,11 +1012,11 @@
   </sheetPr>
   <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="2" sqref="A30 B31 C32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D120" activeCellId="0" sqref="D120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -2050,7 +2050,7 @@
       <c r="A74" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C74" s="0" t="s">
@@ -2075,13 +2075,13 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" s="2" t="s">
         <v>133</v>
       </c>
       <c r="D76" s="0" t="s">
@@ -2246,10 +2246,10 @@
       <c r="A88" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="B88" s="0" t="s">
+      <c r="B88" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C88" s="0" t="s">
+      <c r="C88" s="2" t="s">
         <v>157</v>
       </c>
       <c r="D88" s="0" t="s">
@@ -2257,7 +2257,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B89" s="0" t="s">
@@ -2666,7 +2666,7 @@
       <c r="A118" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B118" s="0" t="s">
+      <c r="B118" s="2" t="s">
         <v>216</v>
       </c>
       <c r="C118" s="0" t="s">
@@ -2700,7 +2700,7 @@
       <c r="C120" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="D120" s="0" t="s">
+      <c r="D120" s="2" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2725,7 +2725,7 @@
       <c r="B122" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="C122" s="0" t="s">
+      <c r="C122" s="2" t="s">
         <v>216</v>
       </c>
       <c r="D122" s="0" t="s">
@@ -2733,7 +2733,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="A123" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B123" s="0" t="s">
@@ -2748,7 +2748,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B124" s="0" t="s">
         <v>224</v>
@@ -2762,21 +2762,21 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C125" s="0" t="s">
         <v>221</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B126" s="0" t="s">
         <v>229</v>
@@ -2790,21 +2790,21 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C127" s="0" t="s">
         <v>224</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>234</v>
@@ -2813,18 +2813,18 @@
         <v>235</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>236</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>137</v>
@@ -2832,13 +2832,13 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>237</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D130" s="0" t="s">
         <v>140</v>
@@ -2846,7 +2846,7 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>238</v>
@@ -2860,7 +2860,7 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>240</v>
@@ -2874,7 +2874,7 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C133" s="0" t="s">
         <v>238</v>
@@ -2885,7 +2885,7 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>240</v>
@@ -2895,17 +2895,14 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
-        <v>238</v>
+      <c r="A135" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="D136" s="0" t="s">
         <v>149</v>
       </c>
@@ -2941,7 +2938,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D143" s="0" t="s">
+      <c r="D143" s="2" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3241,7 +3238,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D203" s="0" t="s">
+      <c r="D203" s="2" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3272,17 +3269,17 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D209" s="0" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D210" s="0" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D211" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3302,7 +3299,7 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D215" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Implement new mathematical commands and enhance dictionary services in Forth runtime
The commit introduces six new mathematical command classes; Times, Divide, TimesDivide, PlusStore, Fetch, and Drop to the Forth runtime. It also adds 'list' functions to the dictionary services for retrieving all repository records. Compatible updates have been made to the ForthInterpreter class to accommodate these enhancements.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="288">
   <si>
     <t xml:space="preserve">Forth-79</t>
   </si>
@@ -91,15 +91,15 @@
     <t xml:space="preserve">(;CODE)</t>
   </si>
   <si>
+    <t xml:space="preserve">-TRAILING</t>
+  </si>
+  <si>
     <t xml:space="preserve">.</t>
   </si>
   <si>
     <t xml:space="preserve">(ABORT)</t>
   </si>
   <si>
-    <t xml:space="preserve">-TRAILING</t>
-  </si>
-  <si>
     <t xml:space="preserve">."</t>
   </si>
   <si>
@@ -136,22 +136,25 @@
     <t xml:space="preserve">1+</t>
   </si>
   <si>
+    <t xml:space="preserve">0&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-</t>
   </si>
   <si>
-    <t xml:space="preserve">0&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">2!</t>
   </si>
   <si>
     <t xml:space="preserve">2*</t>
   </si>
   <si>
+    <t xml:space="preserve">2+</t>
+  </si>
+  <si>
     <t xml:space="preserve">2/</t>
   </si>
   <si>
-    <t xml:space="preserve">2+</t>
+    <t xml:space="preserve">2-</t>
   </si>
   <si>
     <t xml:space="preserve">2@</t>
@@ -160,7 +163,7 @@
     <t xml:space="preserve">+-</t>
   </si>
   <si>
-    <t xml:space="preserve">2-</t>
+    <t xml:space="preserve">79-STANDARD</t>
   </si>
   <si>
     <t xml:space="preserve">2DROP</t>
@@ -169,13 +172,13 @@
     <t xml:space="preserve">+BUF</t>
   </si>
   <si>
-    <t xml:space="preserve">79-STANDARD</t>
+    <t xml:space="preserve">:</t>
   </si>
   <si>
     <t xml:space="preserve">2DUP</t>
   </si>
   <si>
-    <t xml:space="preserve">:</t>
+    <t xml:space="preserve">;</t>
   </si>
   <si>
     <t xml:space="preserve">2OVER</t>
@@ -184,34 +187,34 @@
     <t xml:space="preserve">+ORIGIN</t>
   </si>
   <si>
-    <t xml:space="preserve">;</t>
+    <t xml:space="preserve">&lt;</t>
   </si>
   <si>
     <t xml:space="preserve">2SWAP</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;#</t>
   </si>
   <si>
+    <t xml:space="preserve">&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">--&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;</t>
+    <t xml:space="preserve">&gt;IN</t>
   </si>
   <si>
     <t xml:space="preserve">-DUP</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;IN</t>
+    <t xml:space="preserve">&gt;R</t>
   </si>
   <si>
     <t xml:space="preserve">-FIND</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;R</t>
+    <t xml:space="preserve">?</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;BODY</t>
@@ -220,43 +223,43 @@
     <t xml:space="preserve">-LINE</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
     <t xml:space="preserve">?DUP</t>
   </si>
   <si>
     <t xml:space="preserve">@</t>
   </si>
   <si>
+    <t xml:space="preserve">[</t>
+  </si>
+  <si>
     <t xml:space="preserve">&gt;NUMBER</t>
   </si>
   <si>
-    <t xml:space="preserve">[</t>
+    <t xml:space="preserve">[COMPILE]</t>
   </si>
   <si>
     <t xml:space="preserve">.R</t>
   </si>
   <si>
-    <t xml:space="preserve">[COMPILE]</t>
-  </si>
-  <si>
     <t xml:space="preserve">]</t>
   </si>
   <si>
+    <t xml:space="preserve">ABORT</t>
+  </si>
+  <si>
     <t xml:space="preserve">[']</t>
   </si>
   <si>
-    <t xml:space="preserve">ABORT</t>
-  </si>
-  <si>
     <t xml:space="preserve">ABS</t>
   </si>
   <si>
+    <t xml:space="preserve">ALLOT</t>
+  </si>
+  <si>
     <t xml:space="preserve">MOD</t>
   </si>
   <si>
-    <t xml:space="preserve">ALLOT</t>
+    <t xml:space="preserve">AND</t>
   </si>
   <si>
     <t xml:space="preserve">[CHAR]</t>
@@ -265,22 +268,25 @@
     <t xml:space="preserve">0BRANCH</t>
   </si>
   <si>
-    <t xml:space="preserve">AND</t>
+    <t xml:space="preserve">BASE</t>
   </si>
   <si>
     <t xml:space="preserve">ABORT"</t>
   </si>
   <si>
-    <t xml:space="preserve">BASE</t>
-  </si>
-  <si>
     <t xml:space="preserve">BEGIN</t>
   </si>
   <si>
+    <t xml:space="preserve">BLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOCK</t>
+  </si>
+  <si>
     <t xml:space="preserve">;CODE</t>
   </si>
   <si>
-    <t xml:space="preserve">BLK</t>
+    <t xml:space="preserve">BUFFER</t>
   </si>
   <si>
     <t xml:space="preserve">ACCEPT</t>
@@ -289,36 +295,36 @@
     <t xml:space="preserve">;S</t>
   </si>
   <si>
-    <t xml:space="preserve">BLOCK</t>
+    <t xml:space="preserve">C!</t>
   </si>
   <si>
     <t xml:space="preserve">ALIGN</t>
   </si>
   <si>
-    <t xml:space="preserve">BUFFER</t>
+    <t xml:space="preserve">C@</t>
   </si>
   <si>
     <t xml:space="preserve">ALIGNED</t>
   </si>
   <si>
-    <t xml:space="preserve">C!</t>
+    <t xml:space="preserve">CMOVE</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;BUILDS</t>
   </si>
   <si>
-    <t xml:space="preserve">C@</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMOVE</t>
-  </si>
-  <si>
     <t xml:space="preserve">COLON</t>
   </si>
   <si>
     <t xml:space="preserve">COMPILE</t>
   </si>
   <si>
+    <t xml:space="preserve">CONSTANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTEXT</t>
+  </si>
+  <si>
     <t xml:space="preserve">CMOVE&gt;</t>
   </si>
   <si>
@@ -328,28 +334,28 @@
     <t xml:space="preserve">?COMP</t>
   </si>
   <si>
-    <t xml:space="preserve">CONSTANT</t>
+    <t xml:space="preserve">CONVERT</t>
   </si>
   <si>
     <t xml:space="preserve">?CSP</t>
   </si>
   <si>
+    <t xml:space="preserve">COUNT</t>
+  </si>
+  <si>
     <t xml:space="preserve">C,</t>
   </si>
   <si>
     <t xml:space="preserve">?EXEC</t>
   </si>
   <si>
-    <t xml:space="preserve">CONTEXT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONVERT</t>
+    <t xml:space="preserve">CR</t>
   </si>
   <si>
     <t xml:space="preserve">?LOADING</t>
   </si>
   <si>
-    <t xml:space="preserve">COUNT</t>
+    <t xml:space="preserve">CREATE</t>
   </si>
   <si>
     <t xml:space="preserve">CELL+</t>
@@ -358,7 +364,7 @@
     <t xml:space="preserve">?PAIRS</t>
   </si>
   <si>
-    <t xml:space="preserve">CR</t>
+    <t xml:space="preserve">CURRENT</t>
   </si>
   <si>
     <t xml:space="preserve">CELLS</t>
@@ -367,7 +373,7 @@
     <t xml:space="preserve">?STACK</t>
   </si>
   <si>
-    <t xml:space="preserve">CREATE</t>
+    <t xml:space="preserve">D+</t>
   </si>
   <si>
     <t xml:space="preserve">CHAR</t>
@@ -376,24 +382,18 @@
     <t xml:space="preserve">?TERMINAL</t>
   </si>
   <si>
-    <t xml:space="preserve">D+</t>
+    <t xml:space="preserve">D&lt;</t>
   </si>
   <si>
     <t xml:space="preserve">CHAR+</t>
   </si>
   <si>
-    <t xml:space="preserve">CURRENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D&lt;</t>
+    <t xml:space="preserve">DECIMAL</t>
   </si>
   <si>
     <t xml:space="preserve">CHARS</t>
   </si>
   <si>
-    <t xml:space="preserve">DECIMAL</t>
-  </si>
-  <si>
     <t xml:space="preserve">DEFINITIONS</t>
   </si>
   <si>
@@ -406,28 +406,31 @@
     <t xml:space="preserve">DO</t>
   </si>
   <si>
+    <t xml:space="preserve">DOES&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">AGAIN</t>
   </si>
   <si>
-    <t xml:space="preserve">DOES&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">DROP</t>
   </si>
   <si>
     <t xml:space="preserve">DUP</t>
   </si>
   <si>
+    <t xml:space="preserve">ELSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">B/BUF</t>
   </si>
   <si>
-    <t xml:space="preserve">ELSE</t>
+    <t xml:space="preserve">EMIT</t>
   </si>
   <si>
     <t xml:space="preserve">B/SCR</t>
   </si>
   <si>
-    <t xml:space="preserve">EMIT</t>
+    <t xml:space="preserve">EMPTY-BUFFERS</t>
   </si>
   <si>
     <t xml:space="preserve">BACK</t>
@@ -439,9 +442,6 @@
     <t xml:space="preserve">EXIT</t>
   </si>
   <si>
-    <t xml:space="preserve">EMPTY-BUFFERS</t>
-  </si>
-  <si>
     <t xml:space="preserve">EXPECT</t>
   </si>
   <si>
@@ -460,21 +460,27 @@
     <t xml:space="preserve">FIND</t>
   </si>
   <si>
+    <t xml:space="preserve">FORGET</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLUSH</t>
   </si>
   <si>
-    <t xml:space="preserve">FORGET</t>
+    <t xml:space="preserve">FORTH</t>
   </si>
   <si>
     <t xml:space="preserve">BLOCK-READ</t>
   </si>
   <si>
-    <t xml:space="preserve">FORTH</t>
+    <t xml:space="preserve">HERE</t>
   </si>
   <si>
     <t xml:space="preserve">BLOCK-WRITE</t>
   </si>
   <si>
+    <t xml:space="preserve">HOLD</t>
+  </si>
+  <si>
     <t xml:space="preserve">FORTH-83</t>
   </si>
   <si>
@@ -484,12 +490,6 @@
     <t xml:space="preserve">BRANCH</t>
   </si>
   <si>
-    <t xml:space="preserve">HERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOLD</t>
-  </si>
-  <si>
     <t xml:space="preserve">I</t>
   </si>
   <si>
@@ -499,30 +499,30 @@
     <t xml:space="preserve">IMMEDIATE</t>
   </si>
   <si>
+    <t xml:space="preserve">J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEY</t>
+  </si>
+  <si>
     <t xml:space="preserve">CFA</t>
   </si>
   <si>
-    <t xml:space="preserve">J</t>
+    <t xml:space="preserve">LEAVE</t>
   </si>
   <si>
     <t xml:space="preserve">INVERT</t>
   </si>
   <si>
-    <t xml:space="preserve">KEY</t>
+    <t xml:space="preserve">LIST</t>
   </si>
   <si>
     <t xml:space="preserve">COLD</t>
   </si>
   <si>
-    <t xml:space="preserve">LEAVE</t>
-  </si>
-  <si>
     <t xml:space="preserve">LITERAL</t>
   </si>
   <si>
-    <t xml:space="preserve">LIST</t>
-  </si>
-  <si>
     <t xml:space="preserve">LOAD</t>
   </si>
   <si>
@@ -532,15 +532,18 @@
     <t xml:space="preserve">MAX</t>
   </si>
   <si>
+    <t xml:space="preserve">MIN</t>
+  </si>
+  <si>
     <t xml:space="preserve">LSHIFT</t>
   </si>
   <si>
-    <t xml:space="preserve">MIN</t>
-  </si>
-  <si>
     <t xml:space="preserve">M*</t>
   </si>
   <si>
+    <t xml:space="preserve">MOVE</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSP</t>
   </si>
   <si>
@@ -553,9 +556,6 @@
     <t xml:space="preserve">D+-</t>
   </si>
   <si>
-    <t xml:space="preserve">MOVE</t>
-  </si>
-  <si>
     <t xml:space="preserve">OR</t>
   </si>
   <si>
@@ -577,6 +577,9 @@
     <t xml:space="preserve">PICK</t>
   </si>
   <si>
+    <t xml:space="preserve">QUERY</t>
+  </si>
+  <si>
     <t xml:space="preserve">QUIT</t>
   </si>
   <si>
@@ -595,9 +598,6 @@
     <t xml:space="preserve">DLIST</t>
   </si>
   <si>
-    <t xml:space="preserve">QUERY</t>
-  </si>
-  <si>
     <t xml:space="preserve">REPEAT</t>
   </si>
   <si>
@@ -625,13 +625,22 @@
     <t xml:space="preserve">RSHIFT</t>
   </si>
   <si>
+    <t xml:space="preserve">DP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCR</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPACE</t>
   </si>
   <si>
     <t xml:space="preserve">S"</t>
   </si>
   <si>
-    <t xml:space="preserve">DP</t>
+    <t xml:space="preserve">DPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEMICOLON</t>
   </si>
   <si>
     <t xml:space="preserve">SPACES</t>
@@ -640,16 +649,13 @@
     <t xml:space="preserve">S&gt;D</t>
   </si>
   <si>
-    <t xml:space="preserve">DPL</t>
+    <t xml:space="preserve">DR0</t>
   </si>
   <si>
     <t xml:space="preserve">SPAN</t>
   </si>
   <si>
-    <t xml:space="preserve">DR0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCR</t>
+    <t xml:space="preserve">DR1</t>
   </si>
   <si>
     <t xml:space="preserve">STATE</t>
@@ -658,24 +664,18 @@
     <t xml:space="preserve">SM/REM</t>
   </si>
   <si>
-    <t xml:space="preserve">DR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEMICOLON</t>
-  </si>
-  <si>
     <t xml:space="preserve">SWAP</t>
   </si>
   <si>
     <t xml:space="preserve">SOURCE</t>
   </si>
   <si>
+    <t xml:space="preserve">DUMP</t>
+  </si>
+  <si>
     <t xml:space="preserve">THEN</t>
   </si>
   <si>
-    <t xml:space="preserve">DUMP</t>
-  </si>
-  <si>
     <t xml:space="preserve">TIB</t>
   </si>
   <si>
@@ -685,45 +685,45 @@
     <t xml:space="preserve">U.</t>
   </si>
   <si>
+    <t xml:space="preserve">U*</t>
+  </si>
+  <si>
     <t xml:space="preserve">U&lt;</t>
   </si>
   <si>
+    <t xml:space="preserve">ENCLOSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">UM*</t>
   </si>
   <si>
-    <t xml:space="preserve">ENCLOSE</t>
+    <t xml:space="preserve">END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U/</t>
   </si>
   <si>
     <t xml:space="preserve">UM/MOD</t>
   </si>
   <si>
-    <t xml:space="preserve">END</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U*</t>
+    <t xml:space="preserve">ENDIF</t>
   </si>
   <si>
     <t xml:space="preserve">UNTIL</t>
   </si>
   <si>
-    <t xml:space="preserve">ENDIF</t>
+    <t xml:space="preserve">ERASE</t>
   </si>
   <si>
     <t xml:space="preserve">UPDATE</t>
   </si>
   <si>
-    <t xml:space="preserve">ERASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U/</t>
+    <t xml:space="preserve">ERROR</t>
   </si>
   <si>
     <t xml:space="preserve">VARIABLE</t>
   </si>
   <si>
-    <t xml:space="preserve">ERROR</t>
-  </si>
-  <si>
     <t xml:space="preserve">VOCABULARY</t>
   </si>
   <si>
@@ -733,19 +733,22 @@
     <t xml:space="preserve">WHILE</t>
   </si>
   <si>
+    <t xml:space="preserve">WORDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FENCE</t>
+  </si>
+  <si>
     <t xml:space="preserve">WORD</t>
   </si>
   <si>
     <t xml:space="preserve">XOR</t>
   </si>
   <si>
-    <t xml:space="preserve">FENCE</t>
+    <t xml:space="preserve">FIRST</t>
   </si>
   <si>
     <t xml:space="preserve"> =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIRST</t>
   </si>
   <si>
     <t xml:space="preserve">FLD</t>
@@ -1012,11 +1015,11 @@
   </sheetPr>
   <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D120" activeCellId="0" sqref="D120"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1039,13 +1042,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -1104,7 +1107,7 @@
       <c r="C6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1123,13 +1126,13 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="0" t="s">
@@ -1137,13 +1140,13 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -1154,7 +1157,7 @@
       <c r="A10" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -1179,13 +1182,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -1193,13 +1196,13 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="0" t="s">
@@ -1208,9 +1211,9 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="0" t="s">
@@ -1221,8 +1224,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>19</v>
+      <c r="A15" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>19</v>
@@ -1235,25 +1238,25 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>21</v>
+      <c r="A16" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>26</v>
@@ -1264,12 +1267,12 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="0" t="s">
@@ -1278,7 +1281,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>26</v>
@@ -1292,7 +1295,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>32</v>
@@ -1305,10 +1308,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="A21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1320,7 +1323,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>30</v>
@@ -1328,27 +1331,27 @@
       <c r="C22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
-        <v>39</v>
+      <c r="A24" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>35</v>
@@ -1362,10 +1365,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>41</v>
@@ -1376,195 +1379,195 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C29" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
-        <v>54</v>
+      <c r="A31" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>56</v>
+      <c r="A32" s="0" t="s">
+        <v>57</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>57</v>
+      <c r="A33" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
-        <v>59</v>
+      <c r="A34" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>57</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>67</v>
+      <c r="A38" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>67</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>26</v>
@@ -1572,40 +1575,40 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D42" s="0" t="s">
@@ -1614,13 +1617,13 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>33</v>
@@ -1628,13 +1631,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>35</v>
@@ -1642,24 +1645,24 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>73</v>
@@ -1670,83 +1673,83 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>76</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>84</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>57</v>
@@ -1754,209 +1757,209 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C59" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>107</v>
-      </c>
       <c r="C60" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="C62" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
-        <v>112</v>
+      <c r="A63" s="0" t="s">
+        <v>117</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="D64" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B65" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="C65" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>124</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>73</v>
@@ -1964,27 +1967,27 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>125</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>124</v>
+      <c r="A69" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>126</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>76</v>
@@ -1992,111 +1995,111 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B70" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D70" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="0" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>129</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>125</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="D72" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C72" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="B73" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>130</v>
-      </c>
       <c r="D74" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>131</v>
-      </c>
       <c r="D75" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="2" t="s">
-        <v>133</v>
+      <c r="A76" s="0" t="s">
+        <v>138</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="s">
-        <v>135</v>
+      <c r="A77" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>84</v>
@@ -2104,7 +2107,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>140</v>
@@ -2113,12 +2116,12 @@
         <v>141</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>142</v>
@@ -2132,119 +2135,119 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>145</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>145</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C84" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B86" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="D84" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B85" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="D85" s="0" t="s">
+      <c r="C86" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D86" s="0" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B87" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C87" s="0" t="s">
+      <c r="C87" s="2" t="s">
         <v>156</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>157</v>
@@ -2253,12 +2256,12 @@
         <v>157</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
-        <v>157</v>
+      <c r="A89" s="0" t="s">
+        <v>160</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>158</v>
@@ -2267,46 +2270,46 @@
         <v>158</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B91" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="C91" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B92" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="C92" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="D91" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B92" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>98</v>
@@ -2314,125 +2317,125 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>166</v>
+      <c r="A94" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>167</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D94" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D95" s="0" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B95" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>169</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>168</v>
+        <v>78</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>172</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>169</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B101" s="0" t="s">
         <v>178</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>179</v>
@@ -2440,13 +2443,13 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>180</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>181</v>
@@ -2454,7 +2457,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>182</v>
@@ -2468,7 +2471,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>184</v>
@@ -2477,18 +2480,18 @@
         <v>180</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>124</v>
@@ -2496,41 +2499,41 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>192</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D108" s="0" t="s">
         <v>193</v>
@@ -2538,7 +2541,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B109" s="0" t="s">
         <v>194</v>
@@ -2552,7 +2555,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>197</v>
@@ -2560,13 +2563,13 @@
       <c r="C110" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="D110" s="0" t="s">
+      <c r="D110" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>198</v>
@@ -2575,12 +2578,12 @@
         <v>197</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>199</v>
@@ -2589,68 +2592,68 @@
         <v>200</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>129</v>
+        <v>201</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>199</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="D116" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>214</v>
@@ -2659,54 +2662,54 @@
         <v>215</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>130</v>
+        <v>216</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="D118" s="0" t="s">
-        <v>217</v>
+        <v>203</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>218</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>131</v>
+        <v>207</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
-        <v>204</v>
+      <c r="A120" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>219</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>220</v>
@@ -2714,97 +2717,97 @@
       <c r="C121" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>135</v>
+      <c r="D121" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>139</v>
+        <v>223</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="2" t="s">
-        <v>216</v>
+      <c r="A123" s="0" t="s">
+        <v>220</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C123" s="0" t="s">
         <v>219</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>220</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B127" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="D127" s="0" t="s">
         <v>232</v>
-      </c>
-      <c r="C127" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="D127" s="0" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>234</v>
@@ -2813,458 +2816,458 @@
         <v>235</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>233</v>
+        <v>138</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>236</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="B130" s="0" t="s">
+      <c r="A130" s="2" t="s">
         <v>237</v>
       </c>
+      <c r="B130" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="C130" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>140</v>
+        <v>238</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C131" s="0" t="s">
         <v>236</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>239</v>
+        <v>142</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="B132" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C132" s="0" t="s">
+      <c r="B132" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>237</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>142</v>
+        <v>241</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
-        <v>237</v>
+      <c r="A133" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>242</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="0" t="s">
         <v>240</v>
       </c>
       <c r="D134" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C135" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="D135" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D136" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D137" s="0" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D138" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D139" s="0" t="s">
-        <v>244</v>
+        <v>152</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D140" s="0" t="s">
-        <v>155</v>
+      <c r="D140" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D141" s="0" t="s">
-        <v>156</v>
+        <v>246</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D142" s="0" t="s">
-        <v>245</v>
+      <c r="D142" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D143" s="2" t="s">
-        <v>157</v>
+      <c r="D143" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D144" s="0" t="s">
-        <v>158</v>
+        <v>247</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D145" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D146" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D147" s="0" t="s">
-        <v>248</v>
+        <v>160</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D148" s="0" t="s">
-        <v>162</v>
+        <v>250</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D149" s="0" t="s">
-        <v>249</v>
+        <v>162</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D150" s="0" t="s">
-        <v>164</v>
+        <v>251</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D151" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D152" s="0" t="s">
-        <v>251</v>
+        <v>164</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D153" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D154" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D154" s="0" t="s">
-        <v>252</v>
-      </c>
-    </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D155" s="2" t="s">
-        <v>165</v>
+      <c r="D155" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D156" s="0" t="s">
-        <v>167</v>
+      <c r="D156" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D157" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D158" s="0" t="s">
-        <v>172</v>
+        <v>254</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D159" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D160" s="0" t="s">
-        <v>254</v>
+        <v>169</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D161" s="0" t="s">
-        <v>169</v>
+        <v>256</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D162" s="0" t="s">
-        <v>255</v>
+        <v>170</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D163" s="0" t="s">
-        <v>171</v>
+        <v>257</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D164" s="0" t="s">
-        <v>256</v>
+        <v>78</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D165" s="0" t="s">
-        <v>77</v>
+        <v>258</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D166" s="0" t="s">
-        <v>257</v>
+        <v>173</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D167" s="0" t="s">
-        <v>177</v>
+        <v>259</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D168" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D169" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D170" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D171" s="0" t="s">
-        <v>261</v>
+        <v>178</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D172" s="0" t="s">
-        <v>178</v>
+        <v>263</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D173" s="0" t="s">
-        <v>262</v>
+        <v>180</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D174" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D175" s="0" t="s">
-        <v>182</v>
+        <v>264</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D176" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D177" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D178" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D179" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D180" s="0" t="s">
-        <v>266</v>
+        <v>185</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D181" s="0" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D182" s="0" t="s">
-        <v>185</v>
+        <v>268</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D183" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D184" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D185" s="0" t="s">
-        <v>269</v>
+        <v>188</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D186" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D187" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D188" s="0" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D189" s="0" t="s">
-        <v>197</v>
+        <v>271</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D190" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D191" s="0" t="s">
-        <v>271</v>
+        <v>202</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D192" s="0" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D193" s="0" t="s">
-        <v>199</v>
+        <v>273</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D194" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D195" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D196" s="0" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D197" s="0" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D198" s="0" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D199" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D200" s="0" t="s">
-        <v>214</v>
+        <v>276</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D201" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D202" s="0" t="s">
-        <v>276</v>
+      <c r="D202" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D203" s="2" t="s">
-        <v>216</v>
+      <c r="D203" s="0" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D204" s="0" t="s">
-        <v>218</v>
+        <v>278</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D205" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D206" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D207" s="0" t="s">
-        <v>279</v>
+        <v>219</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D208" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,82 +3277,82 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D210" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D211" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D212" s="0" t="s">
-        <v>229</v>
+        <v>281</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D213" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D214" s="0" t="s">
-        <v>281</v>
+        <v>233</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D215" s="0" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D216" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D217" s="0" t="s">
-        <v>283</v>
+        <v>234</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D218" s="0" t="s">
-        <v>234</v>
+        <v>285</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D219" s="0" t="s">
-        <v>284</v>
+        <v>236</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D220" s="0" t="s">
-        <v>236</v>
+        <v>286</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D221" s="0" t="s">
-        <v>285</v>
+      <c r="D221" s="2" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D222" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D223" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D224" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D225" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new primitive words and corresponding runtime implementation
New primitive words '?dup', 'abort', 'abs', and 'and' have been defined in CoreDefinitions.groovy. Additionally, corresponding runtime classes for each new word have been created with the appropriate execution logic. This expands the available primitive commands users can use in the Forth language interpreter. The 'ForthInterpreter' class was also slightly modified, substituting 'log.debug' with 'log.trace' for word execution logging.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1015,11 +1015,11 @@
   </sheetPr>
   <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D72" activeCellId="0" sqref="D72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1532,7 +1532,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B37" s="0" t="s">
@@ -1563,7 +1563,7 @@
       <c r="A39" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C39" s="0" t="s">
@@ -1594,7 +1594,7 @@
       <c r="B41" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -1602,7 +1602,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B42" s="0" t="s">
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B43" s="0" t="s">
@@ -1644,10 +1644,10 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C45" s="0" t="s">
@@ -1675,10 +1675,10 @@
       <c r="A47" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -1700,7 +1700,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B49" s="0" t="s">
@@ -1745,7 +1745,7 @@
       <c r="A52" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C52" s="0" t="s">
@@ -1776,7 +1776,7 @@
       <c r="B54" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -1975,7 +1975,7 @@
       <c r="C68" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="D68" s="0" t="s">
+      <c r="D68" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1989,7 +1989,7 @@
       <c r="C69" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D69" s="0" t="s">
+      <c r="D69" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2031,7 +2031,7 @@
       <c r="C72" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="D72" s="2" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       <c r="C81" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="D81" s="0" t="s">
+      <c r="D81" s="2" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2288,7 +2288,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="A91" s="2" t="s">
         <v>164</v>
       </c>
       <c r="B91" s="0" t="s">
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="A93" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B93" s="2" t="s">
@@ -2333,7 +2333,7 @@
       <c r="A94" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B94" s="0" t="s">
+      <c r="B94" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C94" s="2" t="s">
@@ -2986,7 +2986,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D152" s="0" t="s">
+      <c r="D152" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D155" s="0" t="s">
+      <c r="D155" s="2" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add CoreMemory class and update Bootstrap class
A new class `CoreMemory` has been added in the 'com.rajames.forth.init' package. This class is initialized within the `Bootstrap` class where some other minor adjustments have been made as well such as including `BlockService`. These changes are expected to enhance the initial system setup and provide a better structure for memory management.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1015,11 +1015,11 @@
   </sheetPr>
   <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D72" activeCellId="0" sqref="D72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1728,7 +1728,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B51" s="0" t="s">
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -1773,7 +1773,7 @@
       <c r="A54" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -1787,7 +1787,7 @@
       <c r="A55" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C55" s="0" t="s">
@@ -1832,7 +1832,7 @@
       <c r="B58" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="2" t="s">
         <v>91</v>
       </c>
       <c r="D58" s="0" t="s">
@@ -1860,7 +1860,7 @@
       <c r="B60" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="2" t="s">
         <v>93</v>
       </c>
       <c r="D60" s="0" t="s">
@@ -2227,7 +2227,7 @@
       <c r="C86" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="D86" s="0" t="s">
+      <c r="D86" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       <c r="C88" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D88" s="0" t="s">
+      <c r="D88" s="2" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new bitwise operator definitions and corresponding classes
This commit builds onto the Forth language runtime by adding definitions for "not", "or", "xor" and "negate" bitwise operators in `CoreDefinitions.groovy`, and the corresponding runtime behavior in their own classes. Additionally, the naming for "COLON" operator has been updated for consistency.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="287">
   <si>
     <t xml:space="preserve">Forth-79</t>
   </si>
@@ -881,9 +881,6 @@
   </si>
   <si>
     <t xml:space="preserve">WIDTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
   </si>
 </sst>
 </file>
@@ -931,7 +928,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -942,6 +939,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -979,7 +982,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -989,6 +992,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1015,11 +1022,11 @@
   </sheetPr>
   <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1056,13 +1063,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -1070,13 +1077,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -1084,13 +1091,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -1098,13 +1105,13 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1112,13 +1119,13 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
@@ -1129,13 +1136,13 @@
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1149,21 +1156,21 @@
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1171,13 +1178,13 @@
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1191,7 +1198,7 @@
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1210,13 +1217,13 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="0" t="s">
@@ -1227,10 +1234,10 @@
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="0" t="s">
@@ -1238,7 +1245,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1255,7 +1262,7 @@
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1286,7 +1293,7 @@
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="0" t="s">
@@ -1294,7 +1301,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="0" t="s">
@@ -1325,10 +1332,10 @@
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1342,7 +1349,7 @@
       <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1350,7 +1357,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1359,12 +1366,12 @@
       <c r="C24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1378,10 +1385,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1392,10 +1399,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="0" t="s">
@@ -1409,7 +1416,7 @@
       <c r="A28" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C28" s="0" t="s">
@@ -1420,10 +1427,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="0" t="s">
@@ -1434,7 +1441,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1451,13 +1458,13 @@
       <c r="A31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1465,10 +1472,10 @@
       <c r="A32" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1482,7 +1489,7 @@
       <c r="B33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D33" s="0" t="s">
@@ -1541,7 +1548,7 @@
       <c r="C37" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1611,7 +1618,7 @@
       <c r="C42" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1667,7 +1674,7 @@
       <c r="C46" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1681,7 +1688,7 @@
       <c r="C47" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1695,7 +1702,7 @@
       <c r="C48" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1770,7 +1777,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -2344,7 +2351,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="2" t="s">
         <v>169</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -2358,10 +2365,10 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="B96" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C96" s="0" t="s">
@@ -2372,10 +2379,10 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C97" s="0" t="s">
@@ -2389,10 +2396,10 @@
       <c r="A98" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C98" s="0" t="s">
+      <c r="C98" s="2" t="s">
         <v>169</v>
       </c>
       <c r="D98" s="0" t="s">
@@ -2400,13 +2407,13 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C99" s="0" t="s">
+      <c r="C99" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D99" s="0" t="s">
@@ -2414,13 +2421,13 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="A100" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B100" s="0" t="s">
+      <c r="B100" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C100" s="0" t="s">
+      <c r="C100" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D100" s="0" t="s">
@@ -2428,10 +2435,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B101" s="0" t="s">
+      <c r="B101" s="2" t="s">
         <v>178</v>
       </c>
       <c r="C101" s="0" t="s">
@@ -2448,7 +2452,7 @@
       <c r="B102" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="C102" s="0" t="s">
+      <c r="C102" s="2" t="s">
         <v>175</v>
       </c>
       <c r="D102" s="0" t="s">
@@ -2462,7 +2466,7 @@
       <c r="B103" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="C103" s="0" t="s">
+      <c r="C103" s="2" t="s">
         <v>178</v>
       </c>
       <c r="D103" s="0" t="s">
@@ -2613,7 +2617,7 @@
       <c r="A114" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="B114" s="0" t="s">
+      <c r="B114" s="2" t="s">
         <v>207</v>
       </c>
       <c r="C114" s="0" t="s">
@@ -2652,10 +2656,10 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="A117" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B117" s="0" t="s">
+      <c r="B117" s="2" t="s">
         <v>214</v>
       </c>
       <c r="C117" s="0" t="s">
@@ -2680,13 +2684,13 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+      <c r="A119" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="C119" s="0" t="s">
+      <c r="C119" s="2" t="s">
         <v>207</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -2714,7 +2718,7 @@
       <c r="B121" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="C121" s="0" t="s">
+      <c r="C121" s="2" t="s">
         <v>214</v>
       </c>
       <c r="D121" s="0" t="s">
@@ -2862,10 +2866,10 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+      <c r="A132" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B132" s="0" t="s">
+      <c r="B132" s="2" t="s">
         <v>240</v>
       </c>
       <c r="C132" s="2" t="s">
@@ -2890,7 +2894,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C134" s="0" t="s">
+      <c r="C134" s="2" t="s">
         <v>240</v>
       </c>
       <c r="D134" s="0" t="s">
@@ -3026,7 +3030,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D160" s="0" t="s">
+      <c r="D160" s="2" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3036,7 +3040,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D162" s="0" t="s">
+      <c r="D162" s="2" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3046,7 +3050,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D164" s="0" t="s">
+      <c r="D164" s="2" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3081,7 +3085,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D171" s="0" t="s">
+      <c r="D171" s="2" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3211,7 +3215,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D197" s="0" t="s">
+      <c r="D197" s="2" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3221,7 +3225,7 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D199" s="0" t="s">
+      <c r="D199" s="2" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3341,8 +3345,8 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D223" s="0" t="s">
-        <v>287</v>
+      <c r="D223" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add comments for future code improvements
In ForthInterpreter.groovy, a comment was added outlining the need for an exception-throwing mechanism for unrecognized words. Comments were also added in ForthRepl.groovy, indicating a future need for serialization on the data and return stacks when implementing a state machine.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -556,27 +556,27 @@
     <t xml:space="preserve">D+-</t>
   </si>
   <si>
+    <t xml:space="preserve">OVER</t>
+  </si>
+  <si>
     <t xml:space="preserve">OR</t>
   </si>
   <si>
     <t xml:space="preserve">D.</t>
   </si>
   <si>
-    <t xml:space="preserve">OVER</t>
+    <t xml:space="preserve">PAD</t>
   </si>
   <si>
     <t xml:space="preserve">D.R</t>
   </si>
   <si>
-    <t xml:space="preserve">PAD</t>
+    <t xml:space="preserve">PICK</t>
   </si>
   <si>
     <t xml:space="preserve">DABS</t>
   </si>
   <si>
-    <t xml:space="preserve">PICK</t>
-  </si>
-  <si>
     <t xml:space="preserve">QUERY</t>
   </si>
   <si>
@@ -619,6 +619,9 @@
     <t xml:space="preserve">SAVE-BUFFERS</t>
   </si>
   <si>
+    <t xml:space="preserve">SCR</t>
+  </si>
+  <si>
     <t xml:space="preserve">SIGN</t>
   </si>
   <si>
@@ -628,7 +631,7 @@
     <t xml:space="preserve">DP</t>
   </si>
   <si>
-    <t xml:space="preserve">SCR</t>
+    <t xml:space="preserve">SEMICOLON</t>
   </si>
   <si>
     <t xml:space="preserve">SPACE</t>
@@ -640,9 +643,6 @@
     <t xml:space="preserve">DPL</t>
   </si>
   <si>
-    <t xml:space="preserve">SEMICOLON</t>
-  </si>
-  <si>
     <t xml:space="preserve">SPACES</t>
   </si>
   <si>
@@ -682,25 +682,28 @@
     <t xml:space="preserve">TYPE</t>
   </si>
   <si>
+    <t xml:space="preserve">U*</t>
+  </si>
+  <si>
     <t xml:space="preserve">U.</t>
   </si>
   <si>
-    <t xml:space="preserve">U*</t>
-  </si>
-  <si>
     <t xml:space="preserve">U&lt;</t>
   </si>
   <si>
     <t xml:space="preserve">ENCLOSE</t>
   </si>
   <si>
+    <t xml:space="preserve">U/</t>
+  </si>
+  <si>
     <t xml:space="preserve">UM*</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
   </si>
   <si>
-    <t xml:space="preserve">U/</t>
+    <t xml:space="preserve">UNTIL</t>
   </si>
   <si>
     <t xml:space="preserve">UM/MOD</t>
@@ -709,46 +712,43 @@
     <t xml:space="preserve">ENDIF</t>
   </si>
   <si>
-    <t xml:space="preserve">UNTIL</t>
+    <t xml:space="preserve">UPDATE</t>
   </si>
   <si>
     <t xml:space="preserve">ERASE</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDATE</t>
+    <t xml:space="preserve">VARIABLE</t>
   </si>
   <si>
     <t xml:space="preserve">ERROR</t>
   </si>
   <si>
-    <t xml:space="preserve">VARIABLE</t>
-  </si>
-  <si>
     <t xml:space="preserve">VOCABULARY</t>
   </si>
   <si>
+    <t xml:space="preserve">WHILE</t>
+  </si>
+  <si>
     <t xml:space="preserve">UNLOOP</t>
   </si>
   <si>
-    <t xml:space="preserve">WHILE</t>
-  </si>
-  <si>
     <t xml:space="preserve">WORDS</t>
   </si>
   <si>
+    <t xml:space="preserve">WORD</t>
+  </si>
+  <si>
     <t xml:space="preserve">FENCE</t>
   </si>
   <si>
-    <t xml:space="preserve">WORD</t>
-  </si>
-  <si>
     <t xml:space="preserve">XOR</t>
   </si>
   <si>
+    <t xml:space="preserve"> =</t>
+  </si>
+  <si>
     <t xml:space="preserve">FIRST</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =</t>
   </si>
   <si>
     <t xml:space="preserve">FLD</t>
@@ -1022,8 +1022,8 @@
   </sheetPr>
   <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2435,53 +2435,56 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="B101" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>173</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>175</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>122</v>
@@ -2489,7 +2492,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>186</v>
@@ -2503,7 +2506,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>188</v>
@@ -2517,7 +2520,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>190</v>
@@ -2531,7 +2534,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>192</v>
@@ -2545,7 +2548,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B109" s="0" t="s">
         <v>194</v>
@@ -2559,7 +2562,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>197</v>
@@ -2573,7 +2576,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>198</v>
@@ -2587,35 +2590,35 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>207</v>
@@ -2629,21 +2632,21 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B115" s="0" t="s">
         <v>210</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D115" s="0" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>203</v>
+      <c r="A116" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="B116" s="0" t="s">
         <v>212</v>
@@ -2656,8 +2659,8 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="2" t="s">
-        <v>207</v>
+      <c r="A117" s="0" t="s">
+        <v>212</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>214</v>
@@ -2670,14 +2673,14 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
-        <v>212</v>
+      <c r="A118" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>217</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>131</v>
@@ -2685,7 +2688,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>218</v>
@@ -2698,8 +2701,8 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="2" t="s">
-        <v>217</v>
+      <c r="A120" s="0" t="s">
+        <v>219</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>219</v>
@@ -2713,10 +2716,10 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>214</v>
@@ -2741,125 +2744,125 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C123" s="0" t="s">
         <v>219</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C125" s="0" t="s">
         <v>222</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="D127" s="0" t="s">
         <v>233</v>
-      </c>
-      <c r="B127" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C127" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D127" s="0" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>234</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
-        <v>236</v>
+      <c r="A129" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="2" t="s">
-        <v>237</v>
+      <c r="A130" s="0" t="s">
+        <v>238</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>237</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D130" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B131" s="0" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B131" s="0" t="s">
-        <v>239</v>
-      </c>
       <c r="C131" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D131" s="0" t="s">
         <v>142</v>
@@ -2867,7 +2870,7 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>240</v>
@@ -2876,18 +2879,15 @@
         <v>237</v>
       </c>
       <c r="D132" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="C133" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>243</v>
@@ -2903,7 +2903,7 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>148</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D171" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,12 +3096,12 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D173" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D174" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,12 +3186,12 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D191" s="0" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D192" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3211,7 +3211,7 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D196" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3271,22 +3271,22 @@
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D208" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D209" s="0" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D210" s="0" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D211" s="0" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3301,7 +3301,7 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D214" s="0" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3326,7 +3326,7 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D219" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3341,7 +3341,7 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D222" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3356,7 +3356,7 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D225" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement multiple runtime classes and update stack interface
Added a series of runtime classes for different operations such as Key, Forget, J, Over, etc., and extended WordRepository and WordService to support deletion of words by creation date. Updated StackInterface in memory package to include a method for getting items from stack. Also, some existing runtime classes and services were updated.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="287">
   <si>
     <t xml:space="preserve">Forth-79</t>
   </si>
@@ -928,7 +928,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,6 +939,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A3FF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -982,7 +988,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -995,11 +1001,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1012,6 +1026,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00A3FF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1020,13 +1094,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D225"/>
+  <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D225" activeCellId="0" sqref="D225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1058,60 +1132,60 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1122,13 +1196,13 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1142,7 +1216,7 @@
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1156,7 +1230,7 @@
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1170,7 +1244,7 @@
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1184,7 +1258,7 @@
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1212,21 +1286,21 @@
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1234,18 +1308,18 @@
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1254,7 +1328,7 @@
       <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1262,13 +1336,13 @@
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1282,7 +1356,7 @@
       <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1296,7 +1370,7 @@
       <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1304,13 +1378,13 @@
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1324,7 +1398,7 @@
       <c r="C21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1335,7 +1409,7 @@
       <c r="B22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1349,7 +1423,7 @@
       <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1357,7 +1431,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1371,7 +1445,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1385,10 +1459,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1399,41 +1473,41 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -1441,16 +1515,16 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1458,24 +1532,24 @@
       <c r="A31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1489,52 +1563,52 @@
       <c r="B33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1542,13 +1616,13 @@
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1556,10 +1630,10 @@
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -1567,13 +1641,13 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -1581,24 +1655,24 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1612,7 +1686,7 @@
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -1626,10 +1700,10 @@
       <c r="A43" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -1637,13 +1711,13 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -1657,29 +1731,29 @@
       <c r="B45" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1688,21 +1762,21 @@
       <c r="C47" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1710,27 +1784,27 @@
       <c r="A49" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1738,10 +1812,10 @@
       <c r="A51" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -1755,24 +1829,24 @@
       <c r="B52" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1791,72 +1865,72 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D59" s="0" t="s">
+      <c r="D59" s="3" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1864,66 +1938,66 @@
       <c r="A60" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="4" t="s">
         <v>104</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D60" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D61" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="D62" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -1931,55 +2005,55 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D66" s="0" t="s">
+      <c r="D66" s="4" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D67" s="0" t="s">
+      <c r="D67" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="2" t="s">
         <v>109</v>
       </c>
       <c r="D68" s="2" t="s">
@@ -1990,10 +2064,10 @@
       <c r="A69" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -2001,16 +2075,16 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" s="3" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2018,13 +2092,13 @@
       <c r="A71" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" s="4" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2049,10 +2123,10 @@
       <c r="B73" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="D73" s="3" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2066,12 +2140,12 @@
       <c r="C74" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D74" s="0" t="s">
+      <c r="D74" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -2080,88 +2154,88 @@
       <c r="C75" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D75" s="0" t="s">
+      <c r="D75" s="3" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="4" t="s">
         <v>138</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D76" s="0" t="s">
+      <c r="D76" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="4" t="s">
         <v>139</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D77" s="0" t="s">
+      <c r="D77" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D78" s="0" t="s">
+      <c r="D78" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="C79" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D79" s="0" t="s">
+      <c r="D79" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="C80" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D80" s="0" t="s">
+      <c r="D80" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C81" s="0" t="s">
+      <c r="C81" s="4" t="s">
         <v>139</v>
       </c>
       <c r="D81" s="2" t="s">
@@ -2169,44 +2243,44 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C82" s="0" t="s">
+      <c r="C82" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D82" s="0" t="s">
+      <c r="D82" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D83" s="0" t="s">
+      <c r="D83" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B84" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D84" s="0" t="s">
+      <c r="D84" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2214,13 +2288,13 @@
       <c r="A85" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="C85" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D85" s="0" t="s">
+      <c r="D85" s="4" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2228,10 +2302,10 @@
       <c r="A86" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C86" s="0" t="s">
+      <c r="C86" s="4" t="s">
         <v>152</v>
       </c>
       <c r="D86" s="2" t="s">
@@ -2239,7 +2313,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="4" t="s">
         <v>158</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -2248,12 +2322,12 @@
       <c r="C87" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D87" s="0" t="s">
+      <c r="D87" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="A88" s="2" t="s">
         <v>159</v>
       </c>
       <c r="B88" s="2" t="s">
@@ -2267,30 +2341,30 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B89" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C89" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D89" s="0" t="s">
+      <c r="D89" s="3" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="B90" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C90" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D90" s="0" t="s">
+      <c r="D90" s="2" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2298,13 +2372,13 @@
       <c r="A91" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="B91" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="C91" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D91" s="0" t="s">
+      <c r="D91" s="3" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2312,13 +2386,13 @@
       <c r="A92" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B92" s="0" t="s">
+      <c r="B92" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C92" s="0" t="s">
+      <c r="C92" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D92" s="0" t="s">
+      <c r="D92" s="4" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2329,10 +2403,10 @@
       <c r="B93" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C93" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D93" s="0" t="s">
+      <c r="C93" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D93" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2346,7 +2420,7 @@
       <c r="C94" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D94" s="0" t="s">
+      <c r="D94" s="4" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2360,7 +2434,7 @@
       <c r="C95" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D95" s="0" t="s">
+      <c r="D95" s="4" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2371,7 +2445,7 @@
       <c r="B96" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C96" s="0" t="s">
+      <c r="C96" s="3" t="s">
         <v>171</v>
       </c>
       <c r="D96" s="2" t="s">
@@ -2385,15 +2459,15 @@
       <c r="B97" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C97" s="0" t="s">
+      <c r="C97" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D97" s="0" t="s">
+      <c r="D97" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B98" s="2" t="s">
@@ -2402,7 +2476,7 @@
       <c r="C98" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D98" s="0" t="s">
+      <c r="D98" s="3" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2416,7 +2490,7 @@
       <c r="C99" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D99" s="0" t="s">
+      <c r="D99" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2430,144 +2504,144 @@
       <c r="C100" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D100" s="0" t="s">
+      <c r="D100" s="4" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+      <c r="A101" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C101" s="0" t="s">
+      <c r="C101" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D101" s="0" t="s">
+      <c r="D101" s="3" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="A102" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="2" t="s">
         <v>178</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D102" s="0" t="s">
+      <c r="D102" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+      <c r="A103" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="4" t="s">
         <v>181</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D103" s="0" t="s">
+      <c r="D103" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+      <c r="A104" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B104" s="0" t="s">
+      <c r="B104" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C104" s="0" t="s">
+      <c r="C104" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D104" s="0" t="s">
+      <c r="D104" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+      <c r="A105" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C105" s="0" t="s">
+      <c r="C105" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D105" s="0" t="s">
+      <c r="D105" s="4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+      <c r="A106" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B106" s="0" t="s">
+      <c r="B106" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C106" s="0" t="s">
+      <c r="C106" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D106" s="0" t="s">
+      <c r="D106" s="3" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+      <c r="A107" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B107" s="0" t="s">
+      <c r="B107" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C107" s="0" t="s">
+      <c r="C107" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D107" s="0" t="s">
+      <c r="D107" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+      <c r="A108" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C108" s="0" t="s">
+      <c r="C108" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D108" s="0" t="s">
+      <c r="D108" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="A109" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C109" s="0" t="s">
+      <c r="C109" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D109" s="0" t="s">
+      <c r="D109" s="3" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="A110" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B110" s="0" t="s">
+      <c r="B110" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C110" s="0" t="s">
+      <c r="C110" s="4" t="s">
         <v>192</v>
       </c>
       <c r="D110" s="2" t="s">
@@ -2575,72 +2649,72 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="A111" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B111" s="0" t="s">
+      <c r="B111" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C111" s="0" t="s">
+      <c r="C111" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D111" s="0" t="s">
+      <c r="D111" s="4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+      <c r="A112" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B112" s="0" t="s">
+      <c r="B112" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C112" s="0" t="s">
+      <c r="C112" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D112" s="0" t="s">
+      <c r="D112" s="3" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+      <c r="A113" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B113" s="0" t="s">
+      <c r="B113" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C113" s="0" t="s">
+      <c r="C113" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D113" s="0" t="s">
+      <c r="D113" s="3" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+      <c r="A114" s="4" t="s">
         <v>200</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C114" s="0" t="s">
+      <c r="C114" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D114" s="0" t="s">
+      <c r="D114" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+      <c r="A115" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B115" s="0" t="s">
+      <c r="B115" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C115" s="0" t="s">
+      <c r="C115" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D115" s="0" t="s">
+      <c r="D115" s="3" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2648,10 +2722,10 @@
       <c r="A116" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B116" s="0" t="s">
+      <c r="B116" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C116" s="0" t="s">
+      <c r="C116" s="3" t="s">
         <v>213</v>
       </c>
       <c r="D116" s="2" t="s">
@@ -2659,16 +2733,16 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="A117" s="4" t="s">
         <v>212</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C117" s="0" t="s">
+      <c r="C117" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D117" s="0" t="s">
+      <c r="D117" s="3" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2679,7 +2753,7 @@
       <c r="B118" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C118" s="0" t="s">
+      <c r="C118" s="2" t="s">
         <v>204</v>
       </c>
       <c r="D118" s="2" t="s">
@@ -2690,7 +2764,7 @@
       <c r="A119" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B119" s="0" t="s">
+      <c r="B119" s="3" t="s">
         <v>218</v>
       </c>
       <c r="C119" s="2" t="s">
@@ -2701,13 +2775,13 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+      <c r="A120" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B120" s="0" t="s">
+      <c r="B120" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C120" s="0" t="s">
+      <c r="C120" s="4" t="s">
         <v>212</v>
       </c>
       <c r="D120" s="2" t="s">
@@ -2715,114 +2789,114 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="A121" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="B121" s="0" t="s">
+      <c r="B121" s="4" t="s">
         <v>221</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D121" s="0" t="s">
+      <c r="D121" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="A122" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B122" s="0" t="s">
+      <c r="B122" s="3" t="s">
         <v>222</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D122" s="0" t="s">
+      <c r="D122" s="3" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="A123" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="B123" s="0" t="s">
+      <c r="B123" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C123" s="0" t="s">
+      <c r="C123" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D123" s="0" t="s">
+      <c r="D123" s="3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="A124" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B124" s="0" t="s">
+      <c r="B124" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="C124" s="0" t="s">
+      <c r="C124" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D124" s="0" t="s">
+      <c r="D124" s="3" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+      <c r="A125" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B125" s="0" t="s">
+      <c r="B125" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C125" s="0" t="s">
+      <c r="C125" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D125" s="0" t="s">
+      <c r="D125" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+      <c r="A126" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B126" s="0" t="s">
+      <c r="B126" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C126" s="0" t="s">
+      <c r="C126" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D126" s="0" t="s">
+      <c r="D126" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
+      <c r="A127" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B127" s="0" t="s">
+      <c r="B127" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C127" s="0" t="s">
+      <c r="C127" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D127" s="0" t="s">
+      <c r="D127" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
+      <c r="A128" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B128" s="0" t="s">
+      <c r="B128" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C128" s="0" t="s">
+      <c r="C128" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D128" s="0" t="s">
+      <c r="D128" s="4" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2830,27 +2904,27 @@
       <c r="A129" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B129" s="0" t="s">
+      <c r="B129" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C129" s="0" t="s">
+      <c r="C129" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="D129" s="0" t="s">
+      <c r="D129" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+      <c r="A130" s="4" t="s">
         <v>238</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C130" s="0" t="s">
+      <c r="C130" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D130" s="0" t="s">
+      <c r="D130" s="3" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2858,13 +2932,13 @@
       <c r="A131" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B131" s="0" t="s">
+      <c r="B131" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C131" s="0" t="s">
+      <c r="C131" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="D131" s="0" t="s">
+      <c r="D131" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2878,7 +2952,7 @@
       <c r="C132" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D132" s="0" t="s">
+      <c r="D132" s="3" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2886,10 +2960,10 @@
       <c r="B133" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C133" s="0" t="s">
+      <c r="C133" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D133" s="0" t="s">
+      <c r="D133" s="3" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2897,7 +2971,7 @@
       <c r="C134" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D134" s="0" t="s">
+      <c r="D134" s="2" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2905,27 +2979,27 @@
       <c r="C135" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D135" s="0" t="s">
+      <c r="D135" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D136" s="0" t="s">
+      <c r="D136" s="4" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D137" s="0" t="s">
+      <c r="D137" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D138" s="0" t="s">
+      <c r="D138" s="3" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D139" s="0" t="s">
+      <c r="D139" s="4" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2935,7 +3009,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D141" s="0" t="s">
+      <c r="D141" s="3" t="s">
         <v>246</v>
       </c>
     </row>
@@ -2945,47 +3019,47 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D143" s="0" t="s">
+      <c r="D143" s="4" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D144" s="0" t="s">
+      <c r="D144" s="3" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D145" s="0" t="s">
+      <c r="D145" s="3" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D146" s="0" t="s">
+      <c r="D146" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D147" s="0" t="s">
+      <c r="D147" s="2" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D148" s="0" t="s">
+      <c r="D148" s="3" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D149" s="0" t="s">
+      <c r="D149" s="4" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D150" s="0" t="s">
+      <c r="D150" s="3" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D151" s="0" t="s">
+      <c r="D151" s="3" t="s">
         <v>252</v>
       </c>
     </row>
@@ -2995,7 +3069,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D153" s="0" t="s">
+      <c r="D153" s="3" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3015,17 +3089,17 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D157" s="0" t="s">
+      <c r="D157" s="3" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D158" s="0" t="s">
+      <c r="D158" s="3" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D159" s="0" t="s">
+      <c r="D159" s="3" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3035,7 +3109,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D161" s="0" t="s">
+      <c r="D161" s="3" t="s">
         <v>256</v>
       </c>
     </row>
@@ -3045,7 +3119,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D163" s="0" t="s">
+      <c r="D163" s="3" t="s">
         <v>257</v>
       </c>
     </row>
@@ -3055,32 +3129,32 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D165" s="0" t="s">
+      <c r="D165" s="3" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D166" s="0" t="s">
+      <c r="D166" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D167" s="0" t="s">
+      <c r="D167" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D168" s="0" t="s">
+      <c r="D168" s="3" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D169" s="0" t="s">
+      <c r="D169" s="3" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D170" s="0" t="s">
+      <c r="D170" s="3" t="s">
         <v>262</v>
       </c>
     </row>
@@ -3090,127 +3164,127 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D172" s="0" t="s">
+      <c r="D172" s="3" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D173" s="0" t="s">
+      <c r="D173" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D174" s="0" t="s">
+      <c r="D174" s="4" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D175" s="0" t="s">
+      <c r="D175" s="3" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D176" s="0" t="s">
+      <c r="D176" s="3" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D177" s="0" t="s">
+      <c r="D177" s="3" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D178" s="0" t="s">
+      <c r="D178" s="3" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D179" s="0" t="s">
+      <c r="D179" s="3" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D180" s="0" t="s">
+      <c r="D180" s="4" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D181" s="0" t="s">
+      <c r="D181" s="2" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D182" s="0" t="s">
+      <c r="D182" s="3" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D183" s="0" t="s">
+      <c r="D183" s="3" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D184" s="0" t="s">
+      <c r="D184" s="3" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D185" s="0" t="s">
+      <c r="D185" s="2" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D186" s="0" t="s">
+      <c r="D186" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D187" s="0" t="s">
+      <c r="D187" s="4" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D188" s="0" t="s">
+      <c r="D188" s="2" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D189" s="0" t="s">
+      <c r="D189" s="3" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D190" s="0" t="s">
+      <c r="D190" s="3" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D191" s="0" t="s">
+      <c r="D191" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D192" s="0" t="s">
+      <c r="D192" s="3" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D193" s="0" t="s">
+      <c r="D193" s="3" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D194" s="0" t="s">
+      <c r="D194" s="3" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D195" s="0" t="s">
+      <c r="D195" s="3" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D196" s="0" t="s">
+      <c r="D196" s="2" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3220,7 +3294,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D198" s="0" t="s">
+      <c r="D198" s="4" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3230,12 +3304,12 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D200" s="0" t="s">
+      <c r="D200" s="3" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D201" s="0" t="s">
+      <c r="D201" s="3" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3245,92 +3319,92 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D203" s="0" t="s">
+      <c r="D203" s="3" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D204" s="0" t="s">
+      <c r="D204" s="3" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D205" s="0" t="s">
+      <c r="D205" s="3" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D206" s="0" t="s">
+      <c r="D206" s="3" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D207" s="0" t="s">
+      <c r="D207" s="4" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D208" s="0" t="s">
+      <c r="D208" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D209" s="0" t="s">
+      <c r="D209" s="3" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D210" s="0" t="s">
+      <c r="D210" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D211" s="0" t="s">
+      <c r="D211" s="3" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D212" s="0" t="s">
+      <c r="D212" s="3" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D213" s="0" t="s">
+      <c r="D213" s="3" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D214" s="0" t="s">
+      <c r="D214" s="3" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D215" s="0" t="s">
+      <c r="D215" s="3" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D216" s="0" t="s">
+      <c r="D216" s="3" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D217" s="0" t="s">
+      <c r="D217" s="4" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D218" s="0" t="s">
+      <c r="D218" s="3" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D219" s="0" t="s">
+      <c r="D219" s="4" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D220" s="0" t="s">
+      <c r="D220" s="3" t="s">
         <v>286</v>
       </c>
     </row>
@@ -3340,7 +3414,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D222" s="0" t="s">
+      <c r="D222" s="4" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3350,12 +3424,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D224" s="0" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D225" s="2" t="s">
+      <c r="D224" s="6" t="s">
         <v>241</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Word fetch/store methods and create new primitive words
Refactored the fetch and store methods in WordRepository to use Long instead of String. Created new primitive words, including "Lit", "Constant", "Variable", and updated some existing ones like "Store" and "Fetch". Updated related service and runtime classes to handle these new and updated primitives.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1096,11 +1096,11 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D225" activeCellId="0" sqref="D225"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D93" activeCellId="0" sqref="D93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1879,7 +1879,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -1924,7 +1924,7 @@
       <c r="A59" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -2025,7 +2025,7 @@
       <c r="B66" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D66" s="4" t="s">
@@ -2406,7 +2406,7 @@
       <c r="C93" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="2" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 'pad' and 'fill' primitive words, update interpreter and compiler
The 'pad' and 'fill' primitive words are added to the runtime and their definitions added to CoreDefinitions. Updates are made to the ForthCompiler, ForthInterpreter, VariableC and Variable classes for better command handling. Peek method is also added to AbstractStack for additional functionality.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1096,11 +1096,11 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D93" activeCellId="0" sqref="D93"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D174" activeCellId="0" sqref="D174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -2201,10 +2201,10 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -2249,7 +2249,7 @@
       <c r="B82" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="2" t="s">
         <v>142</v>
       </c>
       <c r="D82" s="3" t="s">
@@ -2523,7 +2523,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -2540,7 +2540,7 @@
       <c r="A103" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C103" s="2" t="s">
@@ -2938,7 +2938,7 @@
       <c r="C131" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="D131" s="4" t="s">
+      <c r="D131" s="2" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3174,7 +3174,7 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D174" s="4" t="s">
+      <c r="D174" s="2" t="s">
         <v>181</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the runtime package by adding Decimal and Hex classes
These new classes, Decimal and Hex, have been incorporated into the runtime package to handle the conversion of base in the FORTH words "decimal" and "hex". Additionally, these words have also been integrated into CoreDefinitions.groovy to aid in adjusting the base of the FORTH interpreter.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -988,7 +988,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1010,10 +1010,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1096,8 +1092,8 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D174" activeCellId="0" sqref="D174"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D104" activeCellId="0" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1291,13 +1287,13 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1308,7 +1304,7 @@
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1538,7 +1534,7 @@
       <c r="C31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1711,7 +1707,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -1739,7 +1735,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -1770,7 +1766,7 @@
       <c r="A48" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -1784,7 +1780,7 @@
       <c r="A49" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -1843,7 +1839,7 @@
       <c r="B53" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D53" s="3" t="s">
@@ -1871,7 +1867,7 @@
       <c r="B55" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -1949,7 +1945,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -1980,7 +1976,7 @@
       <c r="A63" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -2005,7 +2001,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -2022,7 +2018,7 @@
       <c r="A66" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -2067,7 +2063,7 @@
       <c r="B69" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="2" t="s">
         <v>111</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -2081,7 +2077,7 @@
       <c r="B70" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="2" t="s">
         <v>122</v>
       </c>
       <c r="D70" s="3" t="s">
@@ -2098,7 +2094,7 @@
       <c r="C71" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2168,7 +2164,7 @@
       <c r="C76" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="2" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2187,10 +2183,10 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -2462,7 +2458,7 @@
       <c r="C97" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D97" s="4" t="s">
+      <c r="D97" s="2" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2560,7 +2556,7 @@
       <c r="C104" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="2" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2859,7 +2855,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="2" t="s">
         <v>232</v>
       </c>
       <c r="B126" s="4" t="s">
@@ -2876,7 +2872,7 @@
       <c r="A127" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B127" s="2" t="s">
         <v>232</v>
       </c>
       <c r="C127" s="3" t="s">
@@ -2910,18 +2906,18 @@
       <c r="C129" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="D129" s="4" t="s">
+      <c r="D129" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="4" t="s">
+      <c r="A130" s="2" t="s">
         <v>238</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="C130" s="2" t="s">
         <v>232</v>
       </c>
       <c r="D130" s="3" t="s">
@@ -2932,7 +2928,7 @@
       <c r="A131" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C131" s="4" t="s">
@@ -2960,7 +2956,7 @@
       <c r="B133" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C133" s="4" t="s">
+      <c r="C133" s="2" t="s">
         <v>238</v>
       </c>
       <c r="D133" s="3" t="s">
@@ -3374,7 +3370,7 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D214" s="3" t="s">
+      <c r="D214" s="2" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3414,7 +3410,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D222" s="4" t="s">
+      <c r="D222" s="2" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3424,7 +3420,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D224" s="6" t="s">
+      <c r="D224" s="2" t="s">
         <v>241</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new primitive words and update block handling
Added new primitive words and improved block handling in the Forth Interpreter. New words include ">", "count", "tick", "execute", and "blk". The block number is now updated whenever a block operation is performed, enhancing the efficiency of the Forth interpreter. Also, fixed incorrect setting of 'forthRepl.BASE' in Decimal, Hex, and Base classes.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1093,10 +1093,10 @@
   <dimension ref="A1:D224"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A3:A4 A5"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1133,13 +1133,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3" t="n">
@@ -1147,13 +1147,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="n">
@@ -1161,13 +1161,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="n">
@@ -1175,13 +1175,13 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1192,7 +1192,7 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1212,7 +1212,7 @@
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1240,7 +1240,7 @@
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1254,7 +1254,7 @@
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1539,7 +1539,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1567,10 +1567,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1587,7 +1587,7 @@
       <c r="B35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -1612,7 +1612,7 @@
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -1629,7 +1629,7 @@
       <c r="B38" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -1828,7 +1828,7 @@
       <c r="C52" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -1948,7 +1948,7 @@
       <c r="A61" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C61" s="3" t="s">
@@ -2035,7 +2035,7 @@
       <c r="B67" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="2" t="s">
         <v>106</v>
       </c>
       <c r="D67" s="4" t="s">
@@ -2155,10 +2155,10 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C76" s="2" t="s">
@@ -2217,7 +2217,7 @@
       <c r="B80" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="2" t="s">
         <v>138</v>
       </c>
       <c r="D80" s="4" t="s">
@@ -2430,7 +2430,7 @@
       <c r="C95" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="2" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2892,7 +2892,7 @@
       <c r="C128" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D128" s="4" t="s">
+      <c r="D128" s="2" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Forth Interpreter with new primitive words and block handling
Introduced new primitive words (">", "count", "tick", "execute", "blk") to the Forth Interpreter to enrich its functionality. Improved block handling by updating the block number each time a block operation occurs, increasing overall efficiency. Also tackled a persistent bug with the incorrect setting of 'forthRepl.BASE' in Decimal, Hex, and Base classes.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1092,8 +1092,8 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1763,7 +1763,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -1808,7 +1808,7 @@
       <c r="A51" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2220,7 +2220,7 @@
       <c r="C80" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="2" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add double operations to StackInterface and AbstractStack
Created two double-stack operations (popDouble and pushDouble) in StackInterface and implemented those in AbstractStack. Various 'Double' operations were also added into the CoreDefinitions. Introduced the DoubleUtil utility class in the java file to handle conversion between double precision values to long, and to perform basic mathematical operations such as addition, subtraction, multiplication, division and modulus. This addition improves functionality and allows double numerical operations within the system.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1092,11 +1092,11 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1973,7 +1973,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -1987,10 +1987,10 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -2004,7 +2004,7 @@
       <c r="A65" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -2043,7 +2043,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -2060,7 +2060,7 @@
       <c r="A69" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -2486,7 +2486,7 @@
       <c r="C99" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D99" s="4" t="s">
+      <c r="D99" s="2" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2500,7 +2500,7 @@
       <c r="C100" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D100" s="4" t="s">
+      <c r="D100" s="3" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Comment out compile error in executeWord function
Temporarily suspended the "Compile Only" exception in the ForthInterpreter's executeWord function. Previously, a ForthInterpreterException was thrown if the word in question was marked as compileOnly. This block of code has been commented out under a TODO remark to be revisited later.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1092,11 +1092,11 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D219" activeCellId="0" sqref="D219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1749,7 +1749,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1794,7 +1794,7 @@
       <c r="A50" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -1881,7 +1881,7 @@
       <c r="B56" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -2178,7 +2178,7 @@
       <c r="C77" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="2" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2603,10 +2603,10 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="2" t="s">
         <v>192</v>
       </c>
       <c r="C108" s="2" t="s">
@@ -2637,7 +2637,7 @@
       <c r="B110" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="2" t="s">
         <v>192</v>
       </c>
       <c r="D110" s="2" t="s">
@@ -2827,7 +2827,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="4" t="s">
+      <c r="A124" s="2" t="s">
         <v>227</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -2844,7 +2844,7 @@
       <c r="A125" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="2" t="s">
         <v>227</v>
       </c>
       <c r="C125" s="3" t="s">
@@ -2883,7 +2883,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="4" t="s">
+      <c r="A128" s="2" t="s">
         <v>235</v>
       </c>
       <c r="B128" s="4" t="s">
@@ -2900,7 +2900,7 @@
       <c r="A129" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B129" s="2" t="s">
         <v>235</v>
       </c>
       <c r="C129" s="4" t="s">
@@ -2931,7 +2931,7 @@
       <c r="B131" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C131" s="2" t="s">
         <v>235</v>
       </c>
       <c r="D131" s="2" t="s">
@@ -3235,7 +3235,7 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D187" s="4" t="s">
+      <c r="D187" s="2" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3350,7 +3350,7 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D210" s="3" t="s">
+      <c r="D210" s="2" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3395,7 +3395,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D219" s="4" t="s">
+      <c r="D219" s="2" t="s">
         <v>235</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new bracket related words and refactor getResource method
Addition of new bracket related primitive words ("[", "]", "[compile]") in CoreDefinitions.groovy and the corresponding implementing classes in primitives_classes. In addition, the 'getResource' method is refactored to handle null value by adding the null safe operator. This provides a safer method of handling potential null resource cases, preventing Null Pointer Exceptions.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1092,11 +1092,11 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D219" activeCellId="0" sqref="D219"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D66" activeCellId="0" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1637,7 +1637,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1651,7 +1651,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1665,10 +1665,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1696,10 +1696,10 @@
       <c r="A43" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -1741,7 +1741,7 @@
       <c r="B46" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D46" s="5" t="s">
@@ -2010,7 +2010,7 @@
       <c r="C65" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2024,7 +2024,7 @@
       <c r="C66" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2038,7 +2038,7 @@
       <c r="C67" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="2" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement State enumeration and modify exception handling
A new file, State.groovy, has been created to enumerate the states 'INTERPRET' and 'COMPILE'. This is now being used in ForthCompiler and ForthRepl. Additionally, exception handling in WordService and ForthInterpreter has been modified. Instead of returning null or a comment about exception throwing, now `ForthException` is properly thrown when a word is not found.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1092,11 +1092,11 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D66" activeCellId="0" sqref="D66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -2239,7 +2239,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -2256,7 +2256,7 @@
       <c r="A83" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="2" t="s">
         <v>148</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -2869,7 +2869,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="4" t="s">
+      <c r="A127" s="2" t="s">
         <v>234</v>
       </c>
       <c r="B127" s="2" t="s">
@@ -2886,7 +2886,7 @@
       <c r="A128" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="2" t="s">
         <v>234</v>
       </c>
       <c r="C128" s="3" t="s">
@@ -3385,7 +3385,7 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D217" s="4" t="s">
+      <c r="D217" s="2" t="s">
         <v>234</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement immediate words execution and context management
Added the ability to execute immediate words in ForthCompiler and ForthInterpreter. This also includes the necessary getters and setters for the 'immediate' field in the Word class. Additionally, a new primitive class 'Context' has been introduced for managing vocabulary change context, along with adjusting the 'forget' operation accordingly.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1092,11 +1092,11 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
@@ -1791,7 +1791,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -1836,7 +1836,7 @@
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -1889,7 +1889,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -1959,7 +1959,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -2015,7 +2015,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -2032,7 +2032,7 @@
       <c r="A67" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -2290,7 +2290,7 @@
       <c r="C85" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2351,7 +2351,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -2382,7 +2382,7 @@
       <c r="A92" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C92" s="2" t="s">
@@ -2570,7 +2570,7 @@
       <c r="C105" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D105" s="4" t="s">
+      <c r="D105" s="2" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2645,10 +2645,10 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="2" t="s">
         <v>198</v>
       </c>
       <c r="C111" s="2" t="s">
@@ -3045,7 +3045,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D149" s="4" t="s">
+      <c r="D149" s="2" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement 'Immediate' primitive class in Forth runtime
The new 'Immediate' primitive class has been added to handle the immediate words execution in the Forth runtime system. This includes the creation and registration of 'immediate' word in CoreDefinitions. Also, modifications have been made in the ForthInterpreter to allow the execution of immediate words.
</commit_message>
<xml_diff>
--- a/dox/compare.xlsx
+++ b/dox/compare.xlsx
@@ -1092,8 +1092,8 @@
   </sheetPr>
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D143" activeCellId="0" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2309,7 +2309,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -2340,10 +2340,10 @@
       <c r="A89" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="2" t="s">
         <v>158</v>
       </c>
       <c r="D89" s="3" t="s">
@@ -2673,7 +2673,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -3015,7 +3015,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D143" s="4" t="s">
+      <c r="D143" s="2" t="s">
         <v>158</v>
       </c>
     </row>

</xml_diff>